<commit_message>
Update after class 1
</commit_message>
<xml_diff>
--- a/CSC3510 S2021/Lectures/04 Intro to JUNIT.xlsx
+++ b/CSC3510 S2021/Lectures/04 Intro to JUNIT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Set up" sheetId="2" r:id="rId1"/>
@@ -445,7 +445,7 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>92075</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4784515" cy="405432"/>
+    <xdr:ext cx="6932667" cy="405432"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="9" name="TextBox 8">
@@ -459,8 +459,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10039350" y="803275"/>
-          <a:ext cx="4784515" cy="405432"/>
+          <a:off x="10082893" y="854075"/>
+          <a:ext cx="6932667" cy="405432"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -494,7 +494,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="2000"/>
-            <a:t>Right click here ... then show action context </a:t>
+            <a:t>Right click here...Inside the cup class ... then show action context </a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -770,11 +770,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>377190</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>102870</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="4212563" cy="264560"/>
+      <xdr:colOff>567690</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>143691</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6089809" cy="342786"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="25" name="TextBox 24">
@@ -788,8 +788,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6473190" y="468630"/>
-          <a:ext cx="4212563" cy="264560"/>
+          <a:off x="6690904" y="334191"/>
+          <a:ext cx="6089809" cy="342786"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -822,7 +822,7 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1600"/>
             <a:t>https://www.youtube.com/watch?v=o5pE7L2tVV8 - Brian Fraiser 7:39 </a:t>
           </a:r>
         </a:p>
@@ -872,10 +872,10 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>53975</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="11548161" cy="264560"/>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>81190</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="14648241" cy="311496"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="20" name="TextBox 19">
@@ -889,8 +889,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3409950" y="6276975"/>
-          <a:ext cx="11548161" cy="264560"/>
+          <a:off x="3423557" y="6177190"/>
+          <a:ext cx="14648241" cy="311496"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -923,35 +923,167 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1400"/>
             <a:t>After creating a project ... create a class to test</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:rPr lang="en-US" sz="1400" baseline="0"/>
             <a:t> ... then </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1400"/>
             <a:t> right click the</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:rPr lang="en-US" sz="1400" baseline="0"/>
             <a:t> class </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1400"/>
             <a:t> -&gt; show Context Actions and then -&gt; select Create Tests .... pick JUNIT5</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:rPr lang="en-US" sz="1400" baseline="0"/>
             <a:t> -&gt; Will say not found -&gt; Fix and pick a recent JUNIT5</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US" sz="1400"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>365298</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>85357</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16532679" y="1905000"/>
+          <a:ext cx="5876190" cy="2942857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>68036</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>40821</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>13607</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14464393" y="1211036"/>
+          <a:ext cx="2109107" cy="898071"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>13607</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>394608</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>40821</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Arrow Connector 20"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="11919857" y="1156607"/>
+          <a:ext cx="1333501" cy="789214"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3786,11 +3918,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H103" sqref="H103"/>
+    <sheetView topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AM62" sqref="AM62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3801,11 +3933,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="O46" sqref="O46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3817,11 +3949,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3832,11 +3964,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U164" sqref="U164"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3847,11 +3979,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A145" workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="B145" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>